<commit_message>
fixed experiment pipeline and did some code structure changes
</commit_message>
<xml_diff>
--- a/Results/Master_Results.xlsx
+++ b/Results/Master_Results.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Placeholder" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment_1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experiment_2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Placeholder" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Experiment_2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -453,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,20 +463,10 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>alpha</t>
+          <t>Similarity</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>beta</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Similarity</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Inference_Time</t>
         </is>
@@ -485,75 +474,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>gpt-3.5</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>35.08561825752258</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>alpha</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>beta</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Similarity</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Inference_Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>gpt-3.5</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>32.51587605476379</v>
+      <c r="B2" t="n">
+        <v>837.4010593891144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experiment_v0 is ready to go
</commit_message>
<xml_diff>
--- a/Results/Master_Results.xlsx
+++ b/Results/Master_Results.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Placeholder" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Experiment_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Experiment_1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Experiment_4" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,10 +475,49 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>837.4010593891144</v>
+        <v>17.90007758140564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Similarity</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Inference_Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>193.8237497806549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>